<commit_message>
Added headers to program pages
</commit_message>
<xml_diff>
--- a/Missing info.xlsx
+++ b/Missing info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Engineering\Project log book\Projects\Tool Setup Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Tool Setup Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -229,9 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -239,11 +236,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -301,224 +301,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -939,7 +721,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,26 +742,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1038,7 +820,7 @@
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1076,7 +858,7 @@
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1103,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>5</v>
@@ -1114,7 +896,7 @@
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -1152,7 +934,7 @@
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -1190,7 +972,7 @@
       <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1230,7 +1012,7 @@
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1259,11 +1041,11 @@
       <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>5</v>
@@ -1288,7 +1070,7 @@
       <c r="G10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -1317,7 +1099,7 @@
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1346,7 +1128,7 @@
       <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1375,11 +1157,11 @@
       <c r="G13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>5</v>
@@ -1404,7 +1186,7 @@
       <c r="G14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1433,11 +1215,11 @@
       <c r="G15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>5</v>
@@ -1462,7 +1244,7 @@
       <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -1491,11 +1273,11 @@
       <c r="G17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>5</v>
@@ -1520,11 +1302,11 @@
       <c r="G18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>5</v>
@@ -1549,11 +1331,11 @@
       <c r="G19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>5</v>
@@ -1578,11 +1360,11 @@
       <c r="G20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>5</v>
@@ -1607,11 +1389,11 @@
       <c r="G21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>4</v>
@@ -1625,7 +1407,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="2">
         <v>36</v>
@@ -1636,7 +1418,7 @@
       <c r="G22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -1665,11 +1447,11 @@
       <c r="G23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>5</v>
@@ -1694,11 +1476,11 @@
       <c r="G24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>5</v>
@@ -1723,11 +1505,11 @@
       <c r="G25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>5</v>
@@ -1752,11 +1534,11 @@
       <c r="G26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>5</v>
@@ -1770,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="3">
         <v>50</v>
@@ -1781,7 +1563,7 @@
       <c r="G27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J27" s="1" t="s">
@@ -1810,11 +1592,11 @@
       <c r="G28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>5</v>
@@ -1839,11 +1621,11 @@
       <c r="G29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>5</v>
@@ -1857,7 +1639,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="2">
         <v>56</v>
@@ -1868,11 +1650,11 @@
       <c r="G30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>5</v>
@@ -1897,7 +1679,7 @@
       <c r="G31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="5" t="s">
         <v>39</v>
       </c>
       <c r="J31" s="1" t="s">
@@ -1931,7 +1713,7 @@
       </c>
       <c r="J32" s="2">
         <f>COUNTIF(J3:J31, "y")</f>
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="K32" s="2">
         <f>COUNTIF(K3:K31, "y")</f>
@@ -1946,7 +1728,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
@@ -1970,9 +1752,9 @@
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1984,9 +1766,9 @@
       <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -1998,7 +1780,7 @@
       </c>
       <c r="C36" s="2">
         <f>COUNTIF(C3:C35, "y")</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>